<commit_message>
rewritten the API call,thinking of flattening the entire list of dictionaries for easy access to items written a function for the same
</commit_message>
<xml_diff>
--- a/post_testing/progress.xlsx
+++ b/post_testing/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\singh\Documents\python_rakathon\opensearch_pipeline\post_testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD03656B-9FF9-40B6-975C-56C7D1C3259B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3919F341-7C93-4AC3-AF22-CE09E5D24506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="34776" windowHeight="21096" xr2:uid="{F35F2302-D4D7-4C07-9F86-0807F79AE0A6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Post API Call</t>
   </si>
@@ -78,13 +78,16 @@
   </si>
   <si>
     <t>Done, two added fileds</t>
-  </si>
-  <si>
-    <t>Function will hold list of dictionaries of devices</t>
   </si>
   <si>
     <t>API Tested in Swagger, schematic difference in HES &amp; MDM, HES:     "fromInclusive": true,
     "toInclusive": true Extra</t>
+  </si>
+  <si>
+    <t>Function will hold list of dictionaries of devices, Done for MDM</t>
+  </si>
+  <si>
+    <t>Write the call to run the post API</t>
   </si>
 </sst>
 </file>
@@ -189,8 +192,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{29F535FF-3783-4454-A5BA-27D4026DE693}" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0">
-  <autoFilter ref="A1:D9" xr:uid="{29F535FF-3783-4454-A5BA-27D4026DE693}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{29F535FF-3783-4454-A5BA-27D4026DE693}" name="Table1" displayName="Table1" ref="A1:D10" totalsRowShown="0">
+  <autoFilter ref="A1:D10" xr:uid="{29F535FF-3783-4454-A5BA-27D4026DE693}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{FE866D37-C6C9-4DE0-89BE-5F42ACCEB7AB}" name="Sl No" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{0FC77F40-F8C3-4DB1-BCAF-5F404EBA2F33}" name="Post API Call"/>
@@ -519,10 +522,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D457D668-4386-4339-B58F-947179C42D70}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -558,7 +561,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -589,7 +592,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -597,10 +600,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -611,19 +614,21 @@
         <v>5</v>
       </c>
       <c r="C6" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>6</v>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="1"/>
     </row>
@@ -632,7 +637,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="2" t="b">
         <v>0</v>
@@ -644,12 +649,24 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>